<commit_message>
Update sheets for Billy.
</commit_message>
<xml_diff>
--- a/pub/Wave_Resource_Numbers.xlsx
+++ b/pub/Wave_Resource_Numbers.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lkilcher/Dropbox/work/mhk/wave_res/pub/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51EE9CE7-48DC-5A49-BC5A-CC855BF12299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF71D30B-E80F-F84B-92CF-19281B145B1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="72880" yWindow="23060" windowWidth="28040" windowHeight="17440" xr2:uid="{2D949CA7-6D86-5B46-8670-5AF90C5C93B8}"/>
+    <workbookView xWindow="11960" yWindow="7200" windowWidth="28040" windowHeight="17440" xr2:uid="{2D949CA7-6D86-5B46-8670-5AF90C5C93B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -63,27 +64,12 @@
     <t>Natural</t>
   </si>
   <si>
-    <t>Frac1_Remote</t>
-  </si>
-  <si>
-    <t>Frac1_Natural</t>
-  </si>
-  <si>
     <t>R2</t>
   </si>
   <si>
     <t>Total2</t>
   </si>
   <si>
-    <t>Frac2_Remote</t>
-  </si>
-  <si>
-    <t>Frac2_Natural</t>
-  </si>
-  <si>
-    <t>Frac2_Potential</t>
-  </si>
-  <si>
     <t>TOTAL</t>
   </si>
   <si>
@@ -96,16 +82,34 @@
     <t>(Potential)</t>
   </si>
   <si>
-    <t>Total3</t>
-  </si>
-  <si>
     <t>R3</t>
+  </si>
+  <si>
+    <t>Total3 - TEXT</t>
+  </si>
+  <si>
+    <t>Frac2_Grey</t>
+  </si>
+  <si>
+    <t>Frac2_LightBlue</t>
+  </si>
+  <si>
+    <t>Frac2_DarkBlue</t>
+  </si>
+  <si>
+    <t>Frac1_LightBlue</t>
+  </si>
+  <si>
+    <t>Frac1_DarkBlue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="\+#"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -143,13 +147,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -464,19 +469,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D2BFEEB-0705-5D42-95FD-3C017BDEE645}">
   <dimension ref="A1:R8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="131" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView tabSelected="1" zoomScale="131" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="4" max="5" width="0" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" customWidth="1"/>
     <col min="7" max="7" width="16.1640625" customWidth="1"/>
+    <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
         <v>6</v>
@@ -488,37 +496,37 @@
         <v>8</v>
       </c>
       <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" t="s">
-        <v>11</v>
-      </c>
       <c r="K1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" t="s">
         <v>18</v>
       </c>
-      <c r="L1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" t="s">
-        <v>14</v>
-      </c>
       <c r="O1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
         <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>20</v>
-      </c>
-      <c r="R1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -554,7 +562,7 @@
         <f>SQRT(I2)</f>
         <v>50.497524691810391</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="3">
         <f>L2-E2</f>
         <v>520</v>
       </c>
@@ -612,10 +620,10 @@
         <v>630</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:K8" si="4">SQRT(I3)</f>
+        <f t="shared" ref="J3:J8" si="4">SQRT(I3)</f>
         <v>25.099800796022265</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="3">
         <f t="shared" ref="K3:K7" si="5">L3-E3</f>
         <v>120</v>
       </c>
@@ -675,7 +683,7 @@
         <f t="shared" si="4"/>
         <v>21.679483388678801</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="3">
         <f t="shared" si="5"/>
         <v>90</v>
       </c>
@@ -735,7 +743,7 @@
         <f t="shared" si="4"/>
         <v>18.439088914585774</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="3">
         <f t="shared" si="5"/>
         <v>50</v>
       </c>
@@ -795,7 +803,7 @@
         <f t="shared" si="4"/>
         <v>8.3666002653407556</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="3">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -855,7 +863,7 @@
         <f t="shared" si="4"/>
         <v>5.7445626465380286</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="3">
         <f t="shared" si="5"/>
         <v>16</v>
       </c>
@@ -884,7 +892,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>3300</v>
@@ -915,7 +923,7 @@
         <f t="shared" si="4"/>
         <v>63.953107821277925</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="3">
         <f t="shared" ref="K8" si="10">L8-E8</f>
         <v>790</v>
       </c>

</xml_diff>